<commit_message>
Checking for disabled CPU schedulers #114, disabled DAC #145
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™ CheckID List.xlsx
+++ b/sp_Blitz/sp_Blitz™ CheckID List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="30360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="263">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -833,13 +833,25 @@
   </si>
   <si>
     <t>Drive Space</t>
+  </si>
+  <si>
+    <t>Remote Admin Connections Disabled</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/dac</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/schedulers</t>
+  </si>
+  <si>
+    <t>CPU Schedulers Offline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,6 +888,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -894,11 +914,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -910,8 +932,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1852,13 +1877,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A162" sqref="A162"/>
+      <selection pane="bottomRight" activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4594,7 +4619,38 @@
       </c>
     </row>
     <row r="162" spans="1:5">
-      <c r="E162" s="6"/>
+      <c r="A162" s="4">
+        <v>100</v>
+      </c>
+      <c r="B162" s="5">
+        <v>50</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D162" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="E162" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" s="4">
+        <v>101</v>
+      </c>
+      <c r="B163" s="5">
+        <v>1</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D163" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E163" s="7" t="s">
+        <v>261</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:E161">
@@ -4611,10 +4667,12 @@
     <hyperlink ref="E122" r:id="rId8"/>
     <hyperlink ref="E157" r:id="rId9"/>
     <hyperlink ref="E141" r:id="rId10"/>
+    <hyperlink ref="E162" r:id="rId11"/>
+    <hyperlink ref="E163" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId11"/>
+  <legacyDrawing r:id="rId13"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Checking for databases in unusual states #111
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™ CheckID List.xlsx
+++ b/sp_Blitz/sp_Blitz™ CheckID List.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="264">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -845,6 +845,9 @@
   </si>
   <si>
     <t>CPU Schedulers Offline</t>
+  </si>
+  <si>
+    <t>Databases in Unusual States</t>
   </si>
 </sst>
 </file>
@@ -914,9 +917,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -934,9 +938,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1877,13 +1882,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A164" sqref="A164"/>
+      <selection pane="bottomRight" activeCell="A165" sqref="A165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4650,6 +4655,23 @@
       </c>
       <c r="E163" s="7" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" s="4">
+        <v>102</v>
+      </c>
+      <c r="B164" s="5">
+        <v>20</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D164" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="E164" s="6" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -4669,10 +4691,11 @@
     <hyperlink ref="E141" r:id="rId10"/>
     <hyperlink ref="E162" r:id="rId11"/>
     <hyperlink ref="E163" r:id="rId12"/>
+    <hyperlink ref="E164" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId13"/>
+  <legacyDrawing r:id="rId14"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added #131 checking for virtualization
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™ CheckID List.xlsx
+++ b/sp_Blitz/sp_Blitz™ CheckID List.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="266">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -848,6 +848,12 @@
   </si>
   <si>
     <t>Databases in Unusual States</t>
+  </si>
+  <si>
+    <t>Virtual Server</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/virtual</t>
   </si>
 </sst>
 </file>
@@ -1882,13 +1888,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A165" sqref="A165"/>
+      <selection pane="bottomRight" activeCell="B166" sqref="B166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4672,6 +4678,23 @@
       </c>
       <c r="E164" s="6" t="s">
         <v>238</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" s="4">
+        <v>103</v>
+      </c>
+      <c r="B165" s="5">
+        <v>250</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D165" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="E165" s="6" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -4692,10 +4715,11 @@
     <hyperlink ref="E162" r:id="rId11"/>
     <hyperlink ref="E163" r:id="rId12"/>
     <hyperlink ref="E164" r:id="rId13"/>
+    <hyperlink ref="E165" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId14"/>
+  <legacyDrawing r:id="rId15"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Adding #50 check 104 for control server permissions.
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™ CheckID List.xlsx
+++ b/sp_Blitz/sp_Blitz™ CheckID List.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="267">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -854,6 +854,9 @@
   </si>
   <si>
     <t>http://BrentOzar.com/go/virtual</t>
+  </si>
+  <si>
+    <t>Control Server Permissions</t>
   </si>
 </sst>
 </file>
@@ -923,9 +926,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -944,10 +948,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1888,10 +1893,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B156" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B166" sqref="B166"/>
@@ -4695,6 +4700,23 @@
       </c>
       <c r="E165" s="6" t="s">
         <v>265</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" s="4">
+        <v>104</v>
+      </c>
+      <c r="B166" s="5">
+        <v>10</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D166" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="E166" s="5" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding #24 check 105 for extended stored procs in master
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™ CheckID List.xlsx
+++ b/sp_Blitz/sp_Blitz™ CheckID List.xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="269">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -857,6 +857,12 @@
   </si>
   <si>
     <t>Control Server Permissions</t>
+  </si>
+  <si>
+    <t>Extended Stored Procedures in Master</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/clr</t>
   </si>
 </sst>
 </file>
@@ -1893,13 +1899,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B156" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B151" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B166" sqref="B166"/>
+      <selection pane="bottomRight" activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4717,6 +4723,23 @@
       </c>
       <c r="E166" s="5" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" s="4">
+        <v>105</v>
+      </c>
+      <c r="B167" s="5">
+        <v>50</v>
+      </c>
+      <c r="C167" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D167" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="E167" s="6" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -4738,10 +4761,11 @@
     <hyperlink ref="E163" r:id="rId12"/>
     <hyperlink ref="E164" r:id="rId13"/>
     <hyperlink ref="E165" r:id="rId14"/>
+    <hyperlink ref="E167" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId15"/>
+  <legacyDrawing r:id="rId16"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updating CheckID list for public distribution
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™ CheckID List.xlsx
+++ b/sp_Blitz/sp_Blitz™ CheckID List.xlsx
@@ -26,7 +26,7 @@
     <author>Randy Knight</author>
   </authors>
   <commentList>
-    <comment ref="A129" authorId="0">
+    <comment ref="A132" authorId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="272">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -829,9 +829,6 @@
     <t>http://BrentOzar.com/go/snapshot</t>
   </si>
   <si>
-    <t>Config not running at set value.  Could be anything in sys.configurations</t>
-  </si>
-  <si>
     <t>Drive Space</t>
   </si>
   <si>
@@ -863,13 +860,25 @@
   </si>
   <si>
     <t>http://BrentOzar.com/go/clr</t>
+  </si>
+  <si>
+    <t>sp_Blitz™ Check ID List - v21 April 25, 2013</t>
+  </si>
+  <si>
+    <t>For updates, visit:</t>
+  </si>
+  <si>
+    <t>http://www.BrentOzar.com/blitz/documentation/</t>
+  </si>
+  <si>
+    <t>Config Not Running at Set Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -914,6 +923,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -923,7 +940,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -931,16 +948,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -953,12 +980,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1899,13 +1933,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E167"/>
+  <dimension ref="A1:E170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B151" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A168" sqref="A168"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1913,133 +1947,95 @@
     <col min="1" max="1" width="7.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.5" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="20" thickBot="1">
+      <c r="A1" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickTop="1">
+      <c r="A2" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5">
-        <v>200</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" s="5">
         <v>200</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="5">
         <v>10</v>
@@ -2048,185 +2044,185 @@
         <v>98</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" s="5">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>98</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>12</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5">
+        <v>200</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5">
-        <v>200</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="E10" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="4">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="5">
-        <v>100</v>
-      </c>
       <c r="C11" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>16</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="4">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5">
+        <v>150</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5">
-        <v>100</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="E12" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="4">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>100</v>
+        <v>181</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="4">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" s="5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="4">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="5">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="4">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17" s="5">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>182</v>
+        <v>24</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="4">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18" s="5">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" s="5">
         <v>110</v>
@@ -2235,112 +2231,112 @@
         <v>100</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>149</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="4">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="5">
-        <v>200</v>
+        <v>110</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>37</v>
+        <v>182</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="4">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21" s="5">
         <v>110</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="4">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" s="5">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>212</v>
+        <v>100</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>42</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="4">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" s="5">
         <v>200</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>213</v>
+        <v>37</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>150</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="4">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B24" s="5">
-        <v>200</v>
+        <v>110</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>214</v>
+        <v>39</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>150</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="5">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>101</v>
+        <v>212</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>150</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2354,7 +2350,7 @@
         <v>101</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>44</v>
+        <v>213</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>150</v>
@@ -2371,7 +2367,7 @@
         <v>101</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>45</v>
+        <v>214</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>150</v>
@@ -2388,7 +2384,7 @@
         <v>101</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>226</v>
+        <v>43</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>150</v>
@@ -2405,7 +2401,7 @@
         <v>101</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>225</v>
+        <v>44</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>150</v>
@@ -2422,7 +2418,7 @@
         <v>101</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>150</v>
@@ -2439,7 +2435,7 @@
         <v>101</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>47</v>
+        <v>226</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>150</v>
@@ -2456,7 +2452,7 @@
         <v>101</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>48</v>
+        <v>225</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>150</v>
@@ -2473,7 +2469,7 @@
         <v>101</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>150</v>
@@ -2490,7 +2486,7 @@
         <v>101</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>150</v>
@@ -2507,7 +2503,7 @@
         <v>101</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>150</v>
@@ -2524,7 +2520,7 @@
         <v>101</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>227</v>
+        <v>49</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>150</v>
@@ -2541,7 +2537,7 @@
         <v>101</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>150</v>
@@ -2558,7 +2554,7 @@
         <v>101</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>150</v>
@@ -2575,7 +2571,7 @@
         <v>101</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>54</v>
+        <v>227</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>150</v>
@@ -2592,7 +2588,7 @@
         <v>101</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>150</v>
@@ -2609,7 +2605,7 @@
         <v>101</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>150</v>
@@ -2626,7 +2622,7 @@
         <v>101</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>150</v>
@@ -2643,7 +2639,7 @@
         <v>101</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>150</v>
@@ -2660,7 +2656,7 @@
         <v>101</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>150</v>
@@ -2677,7 +2673,7 @@
         <v>101</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>183</v>
+        <v>57</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>150</v>
@@ -2694,7 +2690,7 @@
         <v>101</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>150</v>
@@ -2711,7 +2707,7 @@
         <v>101</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>150</v>
@@ -2728,7 +2724,7 @@
         <v>101</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>63</v>
+        <v>183</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>150</v>
@@ -2745,7 +2741,7 @@
         <v>101</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>150</v>
@@ -2762,7 +2758,7 @@
         <v>101</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>150</v>
@@ -2779,7 +2775,7 @@
         <v>101</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>150</v>
@@ -2796,7 +2792,7 @@
         <v>101</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>150</v>
@@ -2813,7 +2809,7 @@
         <v>101</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>150</v>
@@ -2830,7 +2826,7 @@
         <v>101</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>150</v>
@@ -2847,7 +2843,7 @@
         <v>101</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>150</v>
@@ -2864,7 +2860,7 @@
         <v>101</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>150</v>
@@ -2881,7 +2877,7 @@
         <v>101</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>150</v>
@@ -2898,7 +2894,7 @@
         <v>101</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>150</v>
@@ -2915,7 +2911,7 @@
         <v>101</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>150</v>
@@ -2932,7 +2928,7 @@
         <v>101</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>150</v>
@@ -2949,7 +2945,7 @@
         <v>101</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>150</v>
@@ -2966,7 +2962,7 @@
         <v>101</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E62" s="5" t="s">
         <v>150</v>
@@ -2983,7 +2979,7 @@
         <v>101</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>150</v>
@@ -3000,7 +2996,7 @@
         <v>101</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>150</v>
@@ -3017,7 +3013,7 @@
         <v>101</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>150</v>
@@ -3034,7 +3030,7 @@
         <v>101</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E66" s="5" t="s">
         <v>150</v>
@@ -3051,7 +3047,7 @@
         <v>101</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>150</v>
@@ -3068,7 +3064,7 @@
         <v>101</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>150</v>
@@ -3085,7 +3081,7 @@
         <v>101</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>150</v>
@@ -3102,7 +3098,7 @@
         <v>101</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>150</v>
@@ -3119,7 +3115,7 @@
         <v>101</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>150</v>
@@ -3136,7 +3132,7 @@
         <v>101</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>150</v>
@@ -3153,7 +3149,7 @@
         <v>101</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E73" s="5" t="s">
         <v>150</v>
@@ -3170,7 +3166,7 @@
         <v>101</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>150</v>
@@ -3187,7 +3183,7 @@
         <v>101</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>150</v>
@@ -3204,7 +3200,7 @@
         <v>101</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>150</v>
@@ -3221,7 +3217,7 @@
         <v>101</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>150</v>
@@ -3238,7 +3234,7 @@
         <v>101</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>215</v>
+        <v>90</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>150</v>
@@ -3255,7 +3251,7 @@
         <v>101</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>216</v>
+        <v>91</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>150</v>
@@ -3272,7 +3268,7 @@
         <v>101</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>150</v>
@@ -3289,7 +3285,7 @@
         <v>101</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>150</v>
@@ -3306,7 +3302,7 @@
         <v>101</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E82" s="5" t="s">
         <v>150</v>
@@ -3323,7 +3319,7 @@
         <v>101</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>150</v>
@@ -3340,7 +3336,7 @@
         <v>101</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>150</v>
@@ -3357,7 +3353,7 @@
         <v>101</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>150</v>
@@ -3374,7 +3370,7 @@
         <v>101</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>221</v>
+        <v>103</v>
       </c>
       <c r="E86" s="5" t="s">
         <v>150</v>
@@ -3391,7 +3387,7 @@
         <v>101</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E87" s="5" t="s">
         <v>150</v>
@@ -3408,7 +3404,7 @@
         <v>101</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>150</v>
@@ -3425,7 +3421,7 @@
         <v>101</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>184</v>
+        <v>221</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>150</v>
@@ -3442,7 +3438,7 @@
         <v>101</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>150</v>
@@ -3459,7 +3455,7 @@
         <v>101</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>104</v>
+        <v>223</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>150</v>
@@ -3467,279 +3463,279 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="4">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B92" s="5">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="4">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B93" s="5">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>187</v>
+        <v>224</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="4">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B94" s="5">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>188</v>
+        <v>104</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="4">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B95" s="5">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="4">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B96" s="5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="4">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B97" s="5">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>228</v>
+        <v>188</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>229</v>
+        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="4">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B98" s="5">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="4">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B99" s="5">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>108</v>
+        <v>190</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="4">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B100" s="5">
-        <v>110</v>
+        <v>200</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>109</v>
+        <v>228</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>154</v>
+        <v>229</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="4">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B101" s="5">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>233</v>
+        <v>99</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="E101" s="6" t="s">
-        <v>235</v>
+        <v>107</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="4">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B102" s="5">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>236</v>
+        <v>99</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="E102" s="6" t="s">
-        <v>238</v>
+        <v>108</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="4">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B103" s="5">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="4">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B104" s="5">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>100</v>
+        <v>233</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>156</v>
+        <v>234</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="4">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B105" s="5">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>100</v>
+        <v>236</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>156</v>
+        <v>237</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="4">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B106" s="5">
+        <v>100</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D106" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C106" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D106" s="5" t="s">
-        <v>111</v>
-      </c>
       <c r="E106" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="4">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B107" s="5">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>112</v>
+        <v>239</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="4">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B108" s="5">
         <v>100</v>
@@ -3748,83 +3744,83 @@
         <v>100</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>113</v>
+        <v>240</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="4">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B109" s="5">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>241</v>
+        <v>111</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>242</v>
+        <v>157</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="4">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B110" s="5">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C110" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>192</v>
+        <v>112</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>193</v>
+        <v>157</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="4">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B111" s="5">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="4">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B112" s="5">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>194</v>
+        <v>241</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>159</v>
+        <v>242</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="4">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B113" s="5">
         <v>100</v>
@@ -3833,66 +3829,66 @@
         <v>100</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>245</v>
+        <v>192</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>246</v>
+        <v>193</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="4">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B114" s="5">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>247</v>
+        <v>114</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>248</v>
+        <v>159</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="4">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B115" s="5">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>115</v>
+        <v>194</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="4">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B116" s="5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>116</v>
+        <v>245</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>161</v>
+        <v>246</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="4">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B117" s="5">
         <v>100</v>
@@ -3901,236 +3897,236 @@
         <v>100</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>117</v>
+        <v>247</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>162</v>
+        <v>248</v>
       </c>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="4">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B118" s="5">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E118" s="6" t="s">
-        <v>162</v>
+        <v>115</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="4">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B119" s="5">
         <v>200</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="4">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B120" s="5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="4">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B121" s="5">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>100</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>160</v>
+        <v>243</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="4">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B122" s="5">
-        <v>10</v>
+        <v>200</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="E122" s="6" t="s">
-        <v>148</v>
+        <v>119</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="4">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B123" s="5">
         <v>200</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>195</v>
+        <v>120</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="4">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B124" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="E124" s="6" t="s">
-        <v>152</v>
+        <v>121</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="4">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B125" s="5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E125" s="5" t="s">
-        <v>165</v>
+        <v>244</v>
+      </c>
+      <c r="E125" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="4">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B126" s="5">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>99</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>124</v>
+        <v>195</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>152</v>
+        <v>196</v>
       </c>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="4">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B127" s="5">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E127" s="5" t="s">
-        <v>166</v>
+        <v>230</v>
+      </c>
+      <c r="E127" s="6" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="4">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B128" s="5">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="4">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B129" s="5">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>251</v>
+        <v>124</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="4">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B130" s="5">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="4">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B131" s="5">
         <v>120</v>
@@ -4139,15 +4135,15 @@
         <v>126</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="4">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B132" s="5">
         <v>120</v>
@@ -4156,134 +4152,134 @@
         <v>126</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>130</v>
+        <v>251</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="4">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B133" s="5">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="4">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B134" s="5">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="4">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B135" s="5">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>199</v>
+        <v>126</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>200</v>
+        <v>130</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>201</v>
+        <v>170</v>
       </c>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="4">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B136" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>252</v>
+        <v>131</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>253</v>
+        <v>171</v>
       </c>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="4">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B137" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="4">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B138" s="5">
         <v>200</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="4">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B139" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>134</v>
+        <v>252</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>174</v>
+        <v>253</v>
       </c>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="4">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B140" s="5">
         <v>50</v>
@@ -4292,66 +4288,66 @@
         <v>99</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>254</v>
+        <v>133</v>
       </c>
       <c r="E140" s="5" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="4">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B141" s="5">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>99</v>
+        <v>202</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E141" s="6" t="s">
-        <v>256</v>
+        <v>203</v>
+      </c>
+      <c r="E141" s="5" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="4">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B142" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E142" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="4">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B143" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>136</v>
+        <v>254</v>
       </c>
       <c r="E143" s="5" t="s">
-        <v>25</v>
+        <v>196</v>
       </c>
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="4">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B144" s="5">
         <v>50</v>
@@ -4360,32 +4356,32 @@
         <v>99</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E144" s="5" t="s">
-        <v>176</v>
+        <v>255</v>
+      </c>
+      <c r="E144" s="6" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="4">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B145" s="5">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>257</v>
+        <v>135</v>
       </c>
       <c r="E145" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="4">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B146" s="5">
         <v>100</v>
@@ -4394,74 +4390,80 @@
         <v>100</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E146" s="5" t="s">
-        <v>178</v>
+        <v>25</v>
       </c>
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="4">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B147" s="5">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
+      </c>
+      <c r="E147" s="5" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="4">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B148" s="5">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>142</v>
+        <v>271</v>
+      </c>
+      <c r="E148" s="5" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="4">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B149" s="5">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
+      </c>
+      <c r="E149" s="5" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="4">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B150" s="5">
-        <v>20</v>
+        <v>250</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>98</v>
+        <v>140</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E150" s="5" t="s">
-        <v>206</v>
+        <v>141</v>
       </c>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="4">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B151" s="5">
         <v>250</v>
@@ -4470,276 +4472,321 @@
         <v>140</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="152" spans="1:5">
       <c r="A152" s="4">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B152" s="5">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>236</v>
+        <v>140</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="E152" s="6" t="s">
-        <v>238</v>
+        <v>143</v>
       </c>
     </row>
     <row r="153" spans="1:5">
       <c r="A153" s="4">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B153" s="5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>236</v>
+        <v>98</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="E153" s="6" t="s">
-        <v>238</v>
+        <v>205</v>
+      </c>
+      <c r="E153" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="4">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B154" s="5">
         <v>250</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>207</v>
+        <v>140</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>258</v>
+        <v>144</v>
       </c>
     </row>
     <row r="155" spans="1:5">
       <c r="A155" s="4">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B155" s="5">
         <v>1</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>97</v>
+        <v>236</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="E155" s="5" t="s">
-        <v>180</v>
+        <v>237</v>
+      </c>
+      <c r="E155" s="6" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="4">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B156" s="5">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>99</v>
+        <v>236</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="E156" s="5" t="s">
-        <v>209</v>
+        <v>237</v>
+      </c>
+      <c r="E156" s="6" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="4">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B157" s="5">
-        <v>110</v>
+        <v>250</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>100</v>
+        <v>207</v>
       </c>
       <c r="D157" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="E157" s="6" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
     </row>
     <row r="158" spans="1:5">
       <c r="A158" s="4">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B158" s="5">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="E158" s="5" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
     </row>
     <row r="159" spans="1:5">
       <c r="A159" s="4">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B159" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D159" s="5" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="E159" s="5" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
     </row>
     <row r="160" spans="1:5">
       <c r="A160" s="4">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B160" s="5">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="E160" s="6" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
     </row>
     <row r="161" spans="1:5">
       <c r="A161" s="4">
+        <v>96</v>
+      </c>
+      <c r="B161" s="5">
+        <v>50</v>
+      </c>
+      <c r="C161" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B161" s="5">
-        <v>110</v>
-      </c>
-      <c r="C161" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="D161" s="5" t="s">
-        <v>210</v>
+        <v>122</v>
       </c>
       <c r="E161" s="5" t="s">
-        <v>211</v>
+        <v>152</v>
       </c>
     </row>
     <row r="162" spans="1:5">
       <c r="A162" s="4">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B162" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D162" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="E162" s="6" t="s">
-        <v>260</v>
+        <v>197</v>
+      </c>
+      <c r="E162" s="5" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="4">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B163" s="5">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D163" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="E163" s="7" t="s">
-        <v>261</v>
+        <v>231</v>
+      </c>
+      <c r="E163" s="6" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="164" spans="1:5">
       <c r="A164" s="4">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B164" s="5">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="E164" s="6" t="s">
-        <v>238</v>
+        <v>210</v>
+      </c>
+      <c r="E164" s="5" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="165" spans="1:5">
       <c r="A165" s="4">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B165" s="5">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E165" s="6" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="166" spans="1:5">
       <c r="A166" s="4">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B166" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="E166" s="5" t="s">
-        <v>147</v>
+        <v>261</v>
+      </c>
+      <c r="E166" s="7" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="167" spans="1:5">
       <c r="A167" s="4">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B167" s="5">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C167" s="5" t="s">
         <v>99</v>
       </c>
       <c r="D167" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E167" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" s="4">
+        <v>103</v>
+      </c>
+      <c r="B168" s="5">
+        <v>250</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="E168" s="6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" s="4">
+        <v>104</v>
+      </c>
+      <c r="B169" s="5">
+        <v>10</v>
+      </c>
+      <c r="C169" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D169" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="E169" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" s="4">
+        <v>105</v>
+      </c>
+      <c r="B170" s="5">
+        <v>50</v>
+      </c>
+      <c r="C170" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D170" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="E170" s="6" t="s">
         <v>267</v>
-      </c>
-      <c r="E167" s="6" t="s">
-        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -4747,25 +4794,26 @@
     <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="E124" r:id="rId1"/>
-    <hyperlink ref="E160" r:id="rId2"/>
-    <hyperlink ref="E101" r:id="rId3"/>
-    <hyperlink ref="E102" r:id="rId4"/>
-    <hyperlink ref="E152" r:id="rId5"/>
-    <hyperlink ref="E153" r:id="rId6"/>
-    <hyperlink ref="E118" r:id="rId7"/>
-    <hyperlink ref="E122" r:id="rId8"/>
-    <hyperlink ref="E157" r:id="rId9"/>
-    <hyperlink ref="E141" r:id="rId10"/>
-    <hyperlink ref="E162" r:id="rId11"/>
-    <hyperlink ref="E163" r:id="rId12"/>
-    <hyperlink ref="E164" r:id="rId13"/>
-    <hyperlink ref="E165" r:id="rId14"/>
-    <hyperlink ref="E167" r:id="rId15"/>
+    <hyperlink ref="E127" r:id="rId1"/>
+    <hyperlink ref="E163" r:id="rId2"/>
+    <hyperlink ref="E104" r:id="rId3"/>
+    <hyperlink ref="E105" r:id="rId4"/>
+    <hyperlink ref="E155" r:id="rId5"/>
+    <hyperlink ref="E156" r:id="rId6"/>
+    <hyperlink ref="E121" r:id="rId7"/>
+    <hyperlink ref="E125" r:id="rId8"/>
+    <hyperlink ref="E160" r:id="rId9"/>
+    <hyperlink ref="E144" r:id="rId10"/>
+    <hyperlink ref="E165" r:id="rId11"/>
+    <hyperlink ref="E166" r:id="rId12"/>
+    <hyperlink ref="E167" r:id="rId13"/>
+    <hyperlink ref="E168" r:id="rId14"/>
+    <hyperlink ref="E170" r:id="rId15"/>
+    <hyperlink ref="C2" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId16"/>
+  <legacyDrawing r:id="rId17"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
v23 added #116, #63, #171, #173
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™ CheckID List.xlsx
+++ b/sp_Blitz/sp_Blitz™ CheckID List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="30360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="278">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -872,6 +872,24 @@
   </si>
   <si>
     <t>Config Not Running at Set Value</t>
+  </si>
+  <si>
+    <t>Default Trace Contents</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/trace</t>
+  </si>
+  <si>
+    <t>Poison Wait Detected: THREADPOOL</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/poison</t>
+  </si>
+  <si>
+    <t>Poison Wait Detected: RESOURCE_SEMAPHORE</t>
+  </si>
+  <si>
+    <t>Poison Wait Detected: RESOURCE_SEMAPHORE_QUERY_COMPILE</t>
   </si>
 </sst>
 </file>
@@ -958,7 +976,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -966,6 +984,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -987,11 +1006,12 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1933,13 +1953,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E170"/>
+  <dimension ref="A1:E174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B127" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="D175" sqref="D175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4787,6 +4807,74 @@
       </c>
       <c r="E170" s="6" t="s">
         <v>267</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" s="4">
+        <v>106</v>
+      </c>
+      <c r="B171" s="5">
+        <v>250</v>
+      </c>
+      <c r="C171" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D171" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="E171" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" s="4">
+        <v>107</v>
+      </c>
+      <c r="B172" s="5">
+        <v>100</v>
+      </c>
+      <c r="C172" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D172" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="E172" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" s="4">
+        <v>108</v>
+      </c>
+      <c r="B173" s="5">
+        <v>100</v>
+      </c>
+      <c r="C173" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D173" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E173" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" s="4">
+        <v>109</v>
+      </c>
+      <c r="B174" s="5">
+        <v>100</v>
+      </c>
+      <c r="C174" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D174" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="E174" s="6" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -4810,10 +4898,14 @@
     <hyperlink ref="E168" r:id="rId14"/>
     <hyperlink ref="E170" r:id="rId15"/>
     <hyperlink ref="C2" r:id="rId16"/>
+    <hyperlink ref="E171" r:id="rId17"/>
+    <hyperlink ref="E172" r:id="rId18"/>
+    <hyperlink ref="E173" r:id="rId19"/>
+    <hyperlink ref="E174" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId17"/>
+  <legacyDrawing r:id="rId21"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Fixing #175, adding check for disabled memory nodes
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™ CheckID List.xlsx
+++ b/sp_Blitz/sp_Blitz™ CheckID List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="279">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -862,9 +862,6 @@
     <t>http://BrentOzar.com/go/clr</t>
   </si>
   <si>
-    <t>sp_Blitz™ Check ID List - v21 April 25, 2013</t>
-  </si>
-  <si>
     <t>For updates, visit:</t>
   </si>
   <si>
@@ -890,6 +887,12 @@
   </si>
   <si>
     <t>Poison Wait Detected: RESOURCE_SEMAPHORE_QUERY_COMPILE</t>
+  </si>
+  <si>
+    <t>Memory Nodes Offline</t>
+  </si>
+  <si>
+    <t>sp_Blitz™ Check ID List - v23 June 19, 2013</t>
   </si>
 </sst>
 </file>
@@ -976,7 +979,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -984,6 +987,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
@@ -1006,12 +1010,13 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1953,13 +1958,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E174"/>
+  <dimension ref="A1:E175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B127" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D175" sqref="D175"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1974,15 +1979,15 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
       <c r="A1" s="8" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1">
       <c r="A2" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>269</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1">
@@ -4444,7 +4449,7 @@
         <v>138</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E148" s="5" t="s">
         <v>177</v>
@@ -4820,10 +4825,10 @@
         <v>140</v>
       </c>
       <c r="D171" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="E171" s="6" t="s">
         <v>272</v>
-      </c>
-      <c r="E171" s="6" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -4837,10 +4842,10 @@
         <v>100</v>
       </c>
       <c r="D172" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E172" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="E172" s="6" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -4854,10 +4859,10 @@
         <v>100</v>
       </c>
       <c r="D173" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E173" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -4871,10 +4876,27 @@
         <v>100</v>
       </c>
       <c r="D174" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E174" s="6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" s="4">
+        <v>110</v>
+      </c>
+      <c r="B175" s="5">
+        <v>1</v>
+      </c>
+      <c r="C175" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D175" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="E174" s="6" t="s">
-        <v>275</v>
+      <c r="E175" s="7" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -4902,10 +4924,11 @@
     <hyperlink ref="E172" r:id="rId18"/>
     <hyperlink ref="E173" r:id="rId19"/>
     <hyperlink ref="E174" r:id="rId20"/>
+    <hyperlink ref="E175" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId21"/>
+  <legacyDrawing r:id="rId22"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added #164 check for full text indexes not populated recently
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz™ CheckID List.xlsx
+++ b/sp_Blitz/sp_Blitz™ CheckID List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26260" windowHeight="23420" activeTab="1"/>
+    <workbookView xWindow="1320" yWindow="900" windowWidth="26260" windowHeight="23420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="285">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -905,6 +905,12 @@
   </si>
   <si>
     <t>http://BrentOzar.com/go/tracking</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/fulltext</t>
+  </si>
+  <si>
+    <t>Full Text Indexes Not Updating</t>
   </si>
 </sst>
 </file>
@@ -1970,13 +1976,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E177"/>
+  <dimension ref="A1:E178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A178" sqref="A178"/>
+      <selection pane="bottomRight" activeCell="D179" sqref="D179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4943,6 +4949,23 @@
       </c>
       <c r="E177" s="6" t="s">
         <v>282</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" s="4">
+        <v>113</v>
+      </c>
+      <c r="B178" s="5">
+        <v>50</v>
+      </c>
+      <c r="C178" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D178" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="E178" s="6" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -4973,10 +4996,11 @@
     <hyperlink ref="E175" r:id="rId21"/>
     <hyperlink ref="E176" r:id="rId22"/>
     <hyperlink ref="E177" r:id="rId23"/>
+    <hyperlink ref="E178" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId24"/>
+  <legacyDrawing r:id="rId25"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>